<commit_message>
contacts page TC done
</commit_message>
<xml_diff>
--- a/src/main/java/InputData/ContactsPageData.xlsx
+++ b/src/main/java/InputData/ContactsPageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>TC No.</t>
   </si>
@@ -36,9 +36,6 @@
     <t>hatgevaibhav69@gmail.com</t>
   </si>
   <si>
-    <t>First  Name</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -48,18 +45,12 @@
     <t>Hatge</t>
   </si>
   <si>
-    <t>Shreyas</t>
-  </si>
-  <si>
     <t>Kolambakar</t>
   </si>
   <si>
     <t>Ankita</t>
   </si>
   <si>
-    <t>Shingre</t>
-  </si>
-  <si>
     <t>Social</t>
   </si>
   <si>
@@ -70,6 +61,39 @@
   </si>
   <si>
     <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Valid First and Last Name</t>
+  </si>
+  <si>
+    <t>First Name is blank</t>
+  </si>
+  <si>
+    <t>Last name is blank</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Vaibhav Hatge</t>
+  </si>
+  <si>
+    <t>The field First Name is required</t>
+  </si>
+  <si>
+    <t>The field Last Name is required</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>First Name</t>
   </si>
 </sst>
 </file>
@@ -115,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -138,12 +162,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -151,6 +199,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,109 +516,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="C3:C4" r:id="rId5" display="Joker@007"/>
-    <hyperlink ref="C3" r:id="rId6"/>
-    <hyperlink ref="C4" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="D3:D4" r:id="rId5" display="Joker@007"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>